<commit_message>
add handlers for adding employy, product
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,30 @@
       <c r="B12" t="inlineStr">
         <is>
           <t>James Smit</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>87654321</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ысаков Акылбек</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Пол полыч</t>
         </is>
       </c>
     </row>
@@ -579,7 +603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,6 +635,33 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Комментарий</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Контроллер</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Акыл</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>